<commit_message>
Inserccion de varios datos
</commit_message>
<xml_diff>
--- a/demosheet.xlsx
+++ b/demosheet.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -366,6 +366,62 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>edad</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sofia</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Carlos</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>